<commit_message>
rmd for glucose treatment stats
</commit_message>
<xml_diff>
--- a/output/GiDietPhys.xlsx
+++ b/output/GiDietPhys.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://usu-my.sharepoint.com/personal/a02308724_aggies_usu_edu/Documents/Desktop/ASU green iguana 2021/greeniguanaAnalysis/output/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="366" documentId="8_{900FFE36-CE08-4829-B466-D22F1D4444E1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{6E1AD763-A0F6-4974-BCF1-542D2A1D0B59}"/>
+  <xr:revisionPtr revIDLastSave="367" documentId="8_{900FFE36-CE08-4829-B466-D22F1D4444E1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{C3D2B8E8-A633-4F65-A704-569227E4D90D}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{C910DBE3-F025-4A65-8898-D5F08109D607}"/>
+    <workbookView xWindow="28680" yWindow="-1470" windowWidth="25440" windowHeight="15390" xr2:uid="{C910DBE3-F025-4A65-8898-D5F08109D607}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="148" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="93" uniqueCount="21">
   <si>
     <t>Water Group</t>
   </si>
@@ -98,18 +98,6 @@
   <si>
     <t>SE</t>
   </si>
-  <si>
-    <t>Δ in water group after diet treatment</t>
-  </si>
-  <si>
-    <t>Δ in dextrose group after diet treatment</t>
-  </si>
-  <si>
-    <t>interpretations</t>
-  </si>
-  <si>
-    <t>Glucose treatment was successful in altering physiological biomarkers in dextrose group for BKA, glucose, glycerol, total triglycerides, true triglycerides and mass. Water group, for obviosu reasons, had unchanged biomarkers. However, when comparing the change in biomarker measurement after diet treatment when comparing across treatment groups, we only found a significant effect in energy metabolites.</t>
-  </si>
 </sst>
 </file>
 
@@ -119,7 +107,7 @@
     <numFmt numFmtId="164" formatCode="0.0"/>
     <numFmt numFmtId="165" formatCode="0.000"/>
   </numFmts>
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -151,13 +139,6 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -305,7 +286,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="54">
+  <cellXfs count="39">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -408,53 +389,8 @@
     <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="1" fontId="1" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="1" fontId="0" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="1" fontId="0" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -772,8 +708,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{82B60E61-B073-46FB-97F3-57E4E75BC566}">
   <dimension ref="A1:BC65"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="G1" workbookViewId="0">
-      <selection activeCell="Q3" sqref="Q3"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="K1" sqref="K1:R34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -789,7 +725,7 @@
     <col min="18" max="18" width="7.26953125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:55" s="3" customFormat="1" ht="72.5" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:55" s="3" customFormat="1" ht="29" x14ac:dyDescent="0.35">
       <c r="A1" s="10"/>
       <c r="B1" s="15"/>
       <c r="C1" s="11" t="s">
@@ -804,22 +740,8 @@
       <c r="H1" s="11"/>
       <c r="I1" s="12"/>
       <c r="J1" s="1"/>
-      <c r="K1" s="39" t="s">
-        <v>18</v>
-      </c>
-      <c r="L1" s="15"/>
-      <c r="M1" s="38" t="s">
-        <v>22</v>
-      </c>
-      <c r="N1" s="46" t="s">
-        <v>21</v>
-      </c>
-      <c r="O1" s="12" t="s">
-        <v>8</v>
-      </c>
-      <c r="P1" s="40"/>
-    </row>
-    <row r="2" spans="1:55" s="3" customFormat="1" ht="43.5" x14ac:dyDescent="0.35">
+    </row>
+    <row r="2" spans="1:55" s="3" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A2" s="10" t="s">
         <v>18</v>
       </c>
@@ -844,25 +766,6 @@
         <v>8</v>
       </c>
       <c r="J2" s="1"/>
-      <c r="K2" s="5" t="s">
-        <v>3</v>
-      </c>
-      <c r="L2" s="16" t="s">
-        <v>1</v>
-      </c>
-      <c r="M2" s="24">
-        <v>-33.345999999999997</v>
-      </c>
-      <c r="N2" s="48">
-        <v>-17.513999999999999</v>
-      </c>
-      <c r="O2" s="47">
-        <v>0.187</v>
-      </c>
-      <c r="P2" s="40"/>
-      <c r="Q2" s="40" t="s">
-        <v>23</v>
-      </c>
     </row>
     <row r="3" spans="1:55" x14ac:dyDescent="0.35">
       <c r="A3" s="5" t="s">
@@ -891,21 +794,6 @@
       </c>
       <c r="I3" s="25">
         <v>0.08</v>
-      </c>
-      <c r="K3" s="7"/>
-      <c r="L3" s="17" t="s">
-        <v>20</v>
-      </c>
-      <c r="M3" s="27">
-        <v>6.2969999999999997</v>
-      </c>
-      <c r="N3" s="28">
-        <v>9.8930000000000007</v>
-      </c>
-      <c r="O3" s="44"/>
-      <c r="P3" s="27"/>
-      <c r="Q3" s="53" t="s">
-        <v>24</v>
       </c>
     </row>
     <row r="4" spans="1:55" x14ac:dyDescent="0.35">
@@ -930,19 +818,6 @@
         <v>5.3</v>
       </c>
       <c r="I4" s="28"/>
-      <c r="K4" s="8"/>
-      <c r="L4" s="18" t="s">
-        <v>2</v>
-      </c>
-      <c r="M4" s="34">
-        <v>18</v>
-      </c>
-      <c r="N4" s="35">
-        <v>18</v>
-      </c>
-      <c r="O4" s="45"/>
-      <c r="P4" s="27"/>
-      <c r="Q4" s="27"/>
     </row>
     <row r="5" spans="1:55" x14ac:dyDescent="0.35">
       <c r="A5" s="8"/>
@@ -966,23 +841,6 @@
         <v>18</v>
       </c>
       <c r="I5" s="30"/>
-      <c r="K5" s="7" t="s">
-        <v>9</v>
-      </c>
-      <c r="L5" s="16" t="s">
-        <v>1</v>
-      </c>
-      <c r="M5" s="27">
-        <v>0.25</v>
-      </c>
-      <c r="N5" s="49">
-        <v>0.46600000000000003</v>
-      </c>
-      <c r="O5" s="47">
-        <v>0.66869999999999996</v>
-      </c>
-      <c r="P5" s="41"/>
-      <c r="Q5" s="27"/>
     </row>
     <row r="6" spans="1:55" x14ac:dyDescent="0.35">
       <c r="A6" s="7" t="s">
@@ -1012,19 +870,6 @@
       <c r="I6" s="21">
         <v>0.19</v>
       </c>
-      <c r="K6" s="7"/>
-      <c r="L6" s="17" t="s">
-        <v>20</v>
-      </c>
-      <c r="M6" s="27">
-        <v>0.36</v>
-      </c>
-      <c r="N6" s="28">
-        <v>0.34300000000000003</v>
-      </c>
-      <c r="O6" s="44"/>
-      <c r="P6" s="27"/>
-      <c r="Q6" s="20"/>
     </row>
     <row r="7" spans="1:55" x14ac:dyDescent="0.35">
       <c r="A7" s="7"/>
@@ -1048,19 +893,6 @@
         <v>0.26900000000000002</v>
       </c>
       <c r="I7" s="21"/>
-      <c r="K7" s="8"/>
-      <c r="L7" s="18" t="s">
-        <v>2</v>
-      </c>
-      <c r="M7" s="34">
-        <v>16</v>
-      </c>
-      <c r="N7" s="35">
-        <v>15</v>
-      </c>
-      <c r="O7" s="45"/>
-      <c r="P7" s="27"/>
-      <c r="Q7" s="20"/>
     </row>
     <row r="8" spans="1:55" x14ac:dyDescent="0.35">
       <c r="A8" s="8"/>
@@ -1085,24 +917,6 @@
       </c>
       <c r="I8" s="22"/>
       <c r="J8" s="6"/>
-      <c r="K8" s="7" t="s">
-        <v>10</v>
-      </c>
-      <c r="L8" s="16" t="s">
-        <v>1</v>
-      </c>
-      <c r="M8" s="27">
-        <v>0.20799999999999999</v>
-      </c>
-      <c r="N8" s="49">
-        <v>0.42199999999999999</v>
-      </c>
-      <c r="O8" s="47">
-        <v>0.70499999999999996</v>
-      </c>
-      <c r="P8" s="41"/>
-      <c r="Q8" s="20"/>
-      <c r="R8" s="6"/>
       <c r="S8" s="6"/>
       <c r="T8" s="6"/>
       <c r="U8" s="6"/>
@@ -1170,20 +984,6 @@
         <v>0.35199999999999998</v>
       </c>
       <c r="J9" s="6"/>
-      <c r="K9" s="7"/>
-      <c r="L9" s="17" t="s">
-        <v>20</v>
-      </c>
-      <c r="M9" s="27">
-        <v>0.34499999999999997</v>
-      </c>
-      <c r="N9" s="28">
-        <v>0.439</v>
-      </c>
-      <c r="O9" s="44"/>
-      <c r="P9" s="27"/>
-      <c r="Q9" s="20"/>
-      <c r="R9" s="6"/>
       <c r="S9" s="6"/>
       <c r="T9" s="6"/>
       <c r="U9" s="6"/>
@@ -1245,20 +1045,6 @@
       </c>
       <c r="I10" s="21"/>
       <c r="J10" s="6"/>
-      <c r="K10" s="8"/>
-      <c r="L10" s="18" t="s">
-        <v>2</v>
-      </c>
-      <c r="M10" s="34">
-        <v>16</v>
-      </c>
-      <c r="N10" s="35">
-        <v>15</v>
-      </c>
-      <c r="O10" s="45"/>
-      <c r="P10" s="27"/>
-      <c r="Q10" s="20"/>
-      <c r="R10" s="6"/>
       <c r="S10" s="6"/>
       <c r="T10" s="6"/>
       <c r="U10" s="6"/>
@@ -1320,24 +1106,6 @@
       </c>
       <c r="I11" s="22"/>
       <c r="J11" s="6"/>
-      <c r="K11" s="7" t="s">
-        <v>11</v>
-      </c>
-      <c r="L11" s="16" t="s">
-        <v>1</v>
-      </c>
-      <c r="M11" s="27">
-        <v>126.833</v>
-      </c>
-      <c r="N11" s="49">
-        <v>47.944000000000003</v>
-      </c>
-      <c r="O11" s="32" t="s">
-        <v>4</v>
-      </c>
-      <c r="P11" s="41"/>
-      <c r="Q11" s="20"/>
-      <c r="R11" s="6"/>
       <c r="S11" s="6"/>
       <c r="T11" s="6"/>
       <c r="U11" s="6"/>
@@ -1405,20 +1173,6 @@
         <v>0.13</v>
       </c>
       <c r="J12" s="6"/>
-      <c r="K12" s="7"/>
-      <c r="L12" s="17" t="s">
-        <v>20</v>
-      </c>
-      <c r="M12" s="27">
-        <v>24.036999999999999</v>
-      </c>
-      <c r="N12" s="28">
-        <v>17.309999999999999</v>
-      </c>
-      <c r="O12" s="44"/>
-      <c r="P12" s="20"/>
-      <c r="Q12" s="20"/>
-      <c r="R12" s="6"/>
       <c r="S12" s="6"/>
       <c r="T12" s="6"/>
       <c r="U12" s="6"/>
@@ -1480,20 +1234,6 @@
       </c>
       <c r="I13" s="21"/>
       <c r="J13" s="6"/>
-      <c r="K13" s="8"/>
-      <c r="L13" s="18" t="s">
-        <v>2</v>
-      </c>
-      <c r="M13" s="34">
-        <v>18</v>
-      </c>
-      <c r="N13" s="35">
-        <v>18</v>
-      </c>
-      <c r="O13" s="45"/>
-      <c r="P13" s="20"/>
-      <c r="Q13" s="20"/>
-      <c r="R13" s="6"/>
       <c r="S13" s="6"/>
       <c r="T13" s="6"/>
       <c r="U13" s="6"/>
@@ -1555,24 +1295,6 @@
       </c>
       <c r="I14" s="22"/>
       <c r="J14" s="6"/>
-      <c r="K14" s="7" t="s">
-        <v>12</v>
-      </c>
-      <c r="L14" s="16" t="s">
-        <v>1</v>
-      </c>
-      <c r="M14" s="27">
-        <v>1.3720000000000001</v>
-      </c>
-      <c r="N14" s="49">
-        <v>0.28660000000000002</v>
-      </c>
-      <c r="O14" s="32" t="s">
-        <v>4</v>
-      </c>
-      <c r="P14" s="41"/>
-      <c r="Q14" s="20"/>
-      <c r="R14" s="6"/>
       <c r="S14" s="6"/>
       <c r="T14" s="6"/>
       <c r="U14" s="6"/>
@@ -1640,20 +1362,6 @@
         <v>4</v>
       </c>
       <c r="J15" s="6"/>
-      <c r="K15" s="7"/>
-      <c r="L15" s="17" t="s">
-        <v>20</v>
-      </c>
-      <c r="M15" s="27">
-        <v>0.436</v>
-      </c>
-      <c r="N15" s="28">
-        <v>7.0000000000000007E-2</v>
-      </c>
-      <c r="O15" s="44"/>
-      <c r="P15" s="37"/>
-      <c r="Q15" s="42"/>
-      <c r="R15" s="6"/>
       <c r="S15" s="6"/>
       <c r="T15" s="6"/>
       <c r="U15" s="6"/>
@@ -1715,20 +1423,6 @@
       </c>
       <c r="I16" s="21"/>
       <c r="J16" s="6"/>
-      <c r="K16" s="8"/>
-      <c r="L16" s="18" t="s">
-        <v>2</v>
-      </c>
-      <c r="M16" s="34">
-        <v>17</v>
-      </c>
-      <c r="N16" s="35">
-        <v>15</v>
-      </c>
-      <c r="O16" s="45"/>
-      <c r="P16" s="37"/>
-      <c r="Q16" s="20"/>
-      <c r="R16" s="6"/>
       <c r="S16" s="6"/>
       <c r="T16" s="6"/>
       <c r="U16" s="6"/>
@@ -1790,24 +1484,6 @@
       </c>
       <c r="I17" s="22"/>
       <c r="J17" s="6"/>
-      <c r="K17" s="7" t="s">
-        <v>13</v>
-      </c>
-      <c r="L17" s="16" t="s">
-        <v>1</v>
-      </c>
-      <c r="M17" s="27">
-        <v>2.536</v>
-      </c>
-      <c r="N17" s="49">
-        <v>-2E-3</v>
-      </c>
-      <c r="O17" s="32" t="s">
-        <v>4</v>
-      </c>
-      <c r="P17" s="41"/>
-      <c r="Q17" s="20"/>
-      <c r="R17" s="6"/>
       <c r="S17" s="6"/>
       <c r="T17" s="6"/>
       <c r="U17" s="6"/>
@@ -1875,20 +1551,6 @@
         <v>0.99</v>
       </c>
       <c r="J18" s="6"/>
-      <c r="K18" s="7"/>
-      <c r="L18" s="17" t="s">
-        <v>20</v>
-      </c>
-      <c r="M18" s="27">
-        <v>0.51800000000000002</v>
-      </c>
-      <c r="N18" s="28">
-        <v>0.17</v>
-      </c>
-      <c r="O18" s="44"/>
-      <c r="P18" s="27"/>
-      <c r="Q18" s="20"/>
-      <c r="R18" s="6"/>
       <c r="S18" s="6"/>
       <c r="T18" s="6"/>
       <c r="U18" s="6"/>
@@ -1950,20 +1612,6 @@
       </c>
       <c r="I19" s="21"/>
       <c r="J19" s="6"/>
-      <c r="K19" s="8"/>
-      <c r="L19" s="18" t="s">
-        <v>2</v>
-      </c>
-      <c r="M19" s="34">
-        <v>17</v>
-      </c>
-      <c r="N19" s="35">
-        <v>15</v>
-      </c>
-      <c r="O19" s="45"/>
-      <c r="P19" s="27"/>
-      <c r="Q19" s="20"/>
-      <c r="R19" s="6"/>
       <c r="S19" s="6"/>
       <c r="T19" s="6"/>
       <c r="U19" s="6"/>
@@ -2025,24 +1673,6 @@
       </c>
       <c r="I20" s="22"/>
       <c r="J20" s="6"/>
-      <c r="K20" s="7" t="s">
-        <v>14</v>
-      </c>
-      <c r="L20" s="16" t="s">
-        <v>1</v>
-      </c>
-      <c r="M20" s="27">
-        <v>1.369</v>
-      </c>
-      <c r="N20" s="48">
-        <v>-0.25600000000000001</v>
-      </c>
-      <c r="O20" s="32" t="s">
-        <v>4</v>
-      </c>
-      <c r="P20" s="41"/>
-      <c r="Q20" s="20"/>
-      <c r="R20" s="6"/>
       <c r="S20" s="6"/>
       <c r="T20" s="6"/>
       <c r="U20" s="6"/>
@@ -2110,20 +1740,6 @@
         <v>0.09</v>
       </c>
       <c r="J21" s="6"/>
-      <c r="K21" s="7"/>
-      <c r="L21" s="17" t="s">
-        <v>20</v>
-      </c>
-      <c r="M21" s="27">
-        <v>0.42699999999999999</v>
-      </c>
-      <c r="N21" s="49">
-        <v>0.14199999999999999</v>
-      </c>
-      <c r="O21" s="44"/>
-      <c r="P21" s="27"/>
-      <c r="Q21" s="20"/>
-      <c r="R21" s="6"/>
       <c r="S21" s="6"/>
       <c r="T21" s="6"/>
       <c r="U21" s="6"/>
@@ -2185,20 +1801,6 @@
       </c>
       <c r="I22" s="21"/>
       <c r="J22" s="6"/>
-      <c r="K22" s="8"/>
-      <c r="L22" s="18" t="s">
-        <v>2</v>
-      </c>
-      <c r="M22" s="34">
-        <v>17</v>
-      </c>
-      <c r="N22" s="50">
-        <v>15</v>
-      </c>
-      <c r="O22" s="45"/>
-      <c r="P22" s="27"/>
-      <c r="Q22" s="20"/>
-      <c r="R22" s="6"/>
       <c r="S22" s="6"/>
       <c r="T22" s="6"/>
       <c r="U22" s="6"/>
@@ -2260,24 +1862,6 @@
       </c>
       <c r="I23" s="22"/>
       <c r="J23" s="6"/>
-      <c r="K23" s="7" t="s">
-        <v>15</v>
-      </c>
-      <c r="L23" s="16" t="s">
-        <v>1</v>
-      </c>
-      <c r="M23" s="27">
-        <v>0.72399999999999998</v>
-      </c>
-      <c r="N23" s="28">
-        <v>-0.64200000000000002</v>
-      </c>
-      <c r="O23" s="47">
-        <v>8.8999999999999996E-2</v>
-      </c>
-      <c r="P23" s="41"/>
-      <c r="Q23" s="20"/>
-      <c r="R23" s="6"/>
       <c r="S23" s="6"/>
       <c r="T23" s="6"/>
       <c r="U23" s="6"/>
@@ -2345,20 +1929,6 @@
         <v>0.25</v>
       </c>
       <c r="J24" s="6"/>
-      <c r="K24" s="7"/>
-      <c r="L24" s="17" t="s">
-        <v>20</v>
-      </c>
-      <c r="M24" s="27">
-        <v>0.55500000000000005</v>
-      </c>
-      <c r="N24" s="28">
-        <v>0.54900000000000004</v>
-      </c>
-      <c r="O24" s="44"/>
-      <c r="P24" s="27"/>
-      <c r="Q24" s="20"/>
-      <c r="R24" s="6"/>
       <c r="S24" s="6"/>
       <c r="T24" s="6"/>
       <c r="U24" s="6"/>
@@ -2420,20 +1990,6 @@
       </c>
       <c r="I25" s="21"/>
       <c r="J25" s="6"/>
-      <c r="K25" s="8"/>
-      <c r="L25" s="18" t="s">
-        <v>2</v>
-      </c>
-      <c r="M25" s="34">
-        <v>18</v>
-      </c>
-      <c r="N25" s="50">
-        <v>17</v>
-      </c>
-      <c r="O25" s="45"/>
-      <c r="P25" s="27"/>
-      <c r="Q25" s="20"/>
-      <c r="R25" s="6"/>
       <c r="S25" s="6"/>
       <c r="T25" s="6"/>
       <c r="U25" s="6"/>
@@ -2495,24 +2051,6 @@
       </c>
       <c r="I26" s="22"/>
       <c r="J26" s="6"/>
-      <c r="K26" s="7" t="s">
-        <v>16</v>
-      </c>
-      <c r="L26" s="16" t="s">
-        <v>1</v>
-      </c>
-      <c r="M26" s="27">
-        <v>-0.37</v>
-      </c>
-      <c r="N26" s="28">
-        <v>0.35</v>
-      </c>
-      <c r="O26" s="47">
-        <v>0.13700000000000001</v>
-      </c>
-      <c r="P26" s="41"/>
-      <c r="Q26" s="20"/>
-      <c r="R26" s="6"/>
       <c r="S26" s="6"/>
       <c r="T26" s="6"/>
       <c r="U26" s="6"/>
@@ -2580,20 +2118,6 @@
         <v>0.314</v>
       </c>
       <c r="J27" s="6"/>
-      <c r="K27" s="7"/>
-      <c r="L27" s="17" t="s">
-        <v>20</v>
-      </c>
-      <c r="M27" s="27">
-        <v>0.33200000000000002</v>
-      </c>
-      <c r="N27" s="28">
-        <v>0.34499999999999997</v>
-      </c>
-      <c r="O27" s="51"/>
-      <c r="P27" s="27"/>
-      <c r="Q27" s="20"/>
-      <c r="R27" s="6"/>
       <c r="S27" s="6"/>
       <c r="T27" s="6"/>
       <c r="U27" s="6"/>
@@ -2655,20 +2179,6 @@
       </c>
       <c r="I28" s="21"/>
       <c r="J28" s="6"/>
-      <c r="K28" s="19"/>
-      <c r="L28" s="18" t="s">
-        <v>2</v>
-      </c>
-      <c r="M28" s="34">
-        <v>18</v>
-      </c>
-      <c r="N28" s="50">
-        <v>17</v>
-      </c>
-      <c r="O28" s="52"/>
-      <c r="P28" s="27"/>
-      <c r="Q28" s="20"/>
-      <c r="R28" s="6"/>
       <c r="S28" s="6"/>
       <c r="T28" s="6"/>
       <c r="U28" s="6"/>
@@ -2730,24 +2240,6 @@
       </c>
       <c r="I29" s="23"/>
       <c r="J29" s="13"/>
-      <c r="K29" s="7" t="s">
-        <v>17</v>
-      </c>
-      <c r="L29" s="16" t="s">
-        <v>1</v>
-      </c>
-      <c r="M29" s="27">
-        <v>0.35299999999999998</v>
-      </c>
-      <c r="N29" s="28">
-        <v>-0.35299999999999998</v>
-      </c>
-      <c r="O29" s="47">
-        <v>0.16800000000000001</v>
-      </c>
-      <c r="P29" s="41"/>
-      <c r="Q29" s="43"/>
-      <c r="R29" s="13"/>
       <c r="S29" s="13"/>
       <c r="T29" s="13"/>
       <c r="U29" s="13"/>
@@ -2815,20 +2307,6 @@
         <v>0.2</v>
       </c>
       <c r="J30" s="6"/>
-      <c r="K30" s="7"/>
-      <c r="L30" s="17" t="s">
-        <v>20</v>
-      </c>
-      <c r="M30" s="27">
-        <v>0.42109999999999997</v>
-      </c>
-      <c r="N30" s="28">
-        <v>0.27</v>
-      </c>
-      <c r="O30" s="51"/>
-      <c r="P30" s="27"/>
-      <c r="Q30" s="20"/>
-      <c r="R30" s="6"/>
       <c r="S30" s="6"/>
       <c r="T30" s="6"/>
       <c r="U30" s="6"/>
@@ -2890,20 +2368,6 @@
       </c>
       <c r="I31" s="21"/>
       <c r="J31" s="6"/>
-      <c r="K31" s="8"/>
-      <c r="L31" s="18" t="s">
-        <v>2</v>
-      </c>
-      <c r="M31" s="34">
-        <v>18</v>
-      </c>
-      <c r="N31" s="50">
-        <v>18</v>
-      </c>
-      <c r="O31" s="52"/>
-      <c r="P31" s="27"/>
-      <c r="Q31" s="20"/>
-      <c r="R31" s="6"/>
       <c r="S31" s="6"/>
       <c r="T31" s="6"/>
       <c r="U31" s="6"/>
@@ -2965,24 +2429,6 @@
       </c>
       <c r="I32" s="22"/>
       <c r="J32" s="6"/>
-      <c r="K32" s="7" t="s">
-        <v>19</v>
-      </c>
-      <c r="L32" s="16" t="s">
-        <v>1</v>
-      </c>
-      <c r="M32" s="27">
-        <v>4.444</v>
-      </c>
-      <c r="N32" s="28">
-        <v>1.0549999999999999</v>
-      </c>
-      <c r="O32" s="32" t="s">
-        <v>4</v>
-      </c>
-      <c r="P32" s="41"/>
-      <c r="Q32" s="20"/>
-      <c r="R32" s="6"/>
       <c r="S32" s="6"/>
       <c r="T32" s="6"/>
       <c r="U32" s="6"/>
@@ -3050,20 +2496,6 @@
         <v>0.39</v>
       </c>
       <c r="J33" s="6"/>
-      <c r="K33" s="7"/>
-      <c r="L33" s="17" t="s">
-        <v>20</v>
-      </c>
-      <c r="M33" s="27">
-        <v>0.98</v>
-      </c>
-      <c r="N33" s="28">
-        <v>1.21</v>
-      </c>
-      <c r="O33" s="51"/>
-      <c r="P33" s="20"/>
-      <c r="Q33" s="20"/>
-      <c r="R33" s="6"/>
       <c r="S33" s="6"/>
       <c r="T33" s="6"/>
       <c r="U33" s="6"/>
@@ -3125,20 +2557,6 @@
       </c>
       <c r="I34" s="21"/>
       <c r="J34" s="6"/>
-      <c r="K34" s="8"/>
-      <c r="L34" s="18" t="s">
-        <v>2</v>
-      </c>
-      <c r="M34" s="34">
-        <v>18</v>
-      </c>
-      <c r="N34" s="50">
-        <v>18</v>
-      </c>
-      <c r="O34" s="45"/>
-      <c r="P34" s="20"/>
-      <c r="Q34" s="20"/>
-      <c r="R34" s="6"/>
       <c r="S34" s="6"/>
       <c r="T34" s="6"/>
       <c r="U34" s="6"/>
@@ -3200,7 +2618,7 @@
       </c>
       <c r="I35" s="22"/>
       <c r="J35" s="6"/>
-      <c r="P35" s="41"/>
+      <c r="P35" s="38"/>
       <c r="Q35" s="20"/>
       <c r="R35" s="6"/>
       <c r="S35" s="6"/>

</xml_diff>